<commit_message>
pdf conversion not working
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/DB/Schedule_template.xlsx
+++ b/WinFormsApp1/WinFormsApp1/DB/Schedule_template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26312"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C70AAB67-0625-4183-9148-F2C987E25C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEC32431-28A5-4BD9-88ED-46DB012A9247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="19020" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -880,8 +880,8 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="A1:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
removed watermark on pdf, installer not updated
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/DB/Schedule_template.xlsx
+++ b/WinFormsApp1/WinFormsApp1/DB/Schedule_template.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26312"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B444B4D5-6069-4869-A776-7209C9F49C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F18439C-3D1B-4D9F-A2AC-069806AFD5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="19020" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="19020" windowHeight="13680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly schedule" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Time / period</t>
   </si>
@@ -97,6 +98,9 @@
   </si>
   <si>
     <t>9PM</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -925,7 +929,7 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1151,4 +1155,24 @@
   <pageSetup scale="97" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B050A178-1FFB-4C05-978F-81338794AD70}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>